<commit_message>
Support extended #ignore functionality in progbooks, update documentation and version
</commit_message>
<xml_diff>
--- a/docs/tutorial/assets/T1/t1_databook_1.xlsx
+++ b/docs/tutorial/assets/T1/t1_databook_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\docs\tutorial\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romesh\projects\atomica\docs\tutorial\assets\T1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2203A87-EC8A-479D-A719-CDDEA24669CC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5127D94C-88CB-4817-A1B7-05EA1792E1D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="75" windowWidth="21225" windowHeight="17085" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="4065" windowWidth="32370" windowHeight="15690" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -105,7 +110,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +122,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -143,14 +162,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -193,8 +210,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -208,10 +227,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
@@ -289,9 +310,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -329,9 +350,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -364,26 +385,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -416,26 +420,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -747,10 +734,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="Q5" sqref="Q5:Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,7 +750,7 @@
     <col min="6" max="7" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -784,7 +771,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>adults</v>
@@ -802,7 +789,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -822,13 +809,15 @@
       <c r="G4" s="1">
         <v>2017</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="5" t="s">
+      <c r="H4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>adults</v>
@@ -845,11 +834,13 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -873,7 +864,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>adults</v>
@@ -896,7 +887,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -917,7 +908,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>adults</v>
@@ -934,31 +925,29 @@
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -979,7 +968,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>adults</v>
@@ -998,44 +987,44 @@
       <c r="G15" s="2"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="expression" dxfId="9" priority="1">
+      <formula>COUNTIF(F2:G2,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="2">
+      <formula>AND(COUNTIF(F2:G2,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="expression" dxfId="7" priority="3">
+      <formula>COUNTIF(F5:G5,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="4">
+      <formula>AND(COUNTIF(F5:G5,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>COUNTIF(F8:G8,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>AND(COUNTIF(F8:G8,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="9" priority="7">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>COUNTIF(F11:G11,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="2" priority="8">
       <formula>AND(COUNTIF(F11:G11,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="expression" dxfId="7" priority="9">
+    <cfRule type="expression" dxfId="1" priority="9">
       <formula>COUNTIF(F15:G15,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="10">
+    <cfRule type="expression" dxfId="0" priority="10">
       <formula>AND(COUNTIF(F15:G15,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="5" priority="1">
-      <formula>COUNTIF(F2:G2,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
-      <formula>AND(COUNTIF(F2:G2,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>COUNTIF(F5:G5,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>AND(COUNTIF(F5:G5,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
-    <cfRule type="expression" dxfId="1" priority="5">
-      <formula>COUNTIF(F8:G8,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="6">
-      <formula>AND(COUNTIF(F8:G8,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">

</xml_diff>